<commit_message>
PROS-6604 - MARSRU - KPIs 2019
</commit_message>
<xml_diff>
--- a/Projects/MARSRU_PROD/Data/2019/MARS KPIs.xlsx
+++ b/Projects/MARSRU_PROD/Data/2019/MARS KPIs.xlsx
@@ -48,13 +48,15 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPI!$A$1:$Y$53</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPI!$A$1:$Y$53</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPI!$A$1:$Y$53</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPI!$A$1:$Y$53</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'4317'!$A$1:$C$54</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">'4254'!$A$1:$J$259</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">'4254'!$A$1:$J$259</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'4254'!$A$2:$J$260</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'4254'!$A$1:$J$259</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">'4254'!$A$2:$J$260</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'4254'!$A$1:$J$259</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">'4254'!$A$2:$J$260</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">'4254'!$A$1:$J$259</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">'4254'!$A$2:$J$260</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">'4254'!$A$2:$J$260</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -1556,29 +1558,29 @@
   </sheetPr>
   <dimension ref="1:53"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="64" zoomScaleNormal="64" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="O52" activeCellId="0" sqref="O52"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="64" zoomScaleNormal="64" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
+      <selection pane="bottomLeft" activeCell="H44" activeCellId="0" sqref="H44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="21.7449392712551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="21.9595141700405"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="2" width="8.03238866396761"/>
     <col collapsed="false" hidden="false" max="4" min="3" style="2" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="3" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="3" width="38.3481781376518"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="4" width="43.0607287449393"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="5" width="100.048582995951"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="29.7773279352227"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="3" width="16.0688259109312"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="3" width="38.668016194332"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="4" width="43.4898785425101"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="5" width="100.906882591093"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="29.9919028340081"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="3" width="16.1740890688259"/>
     <col collapsed="false" hidden="false" max="14" min="11" style="2" width="8.89068825910931"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="6" width="28.4939271255061"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="3" width="16.0688259109312"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="6" width="28.7085020242915"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="3" width="16.1740890688259"/>
     <col collapsed="false" hidden="false" max="23" min="17" style="3" width="13.6032388663968"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="3" width="18.5303643724696"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="5" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="3" width="18.6396761133603"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="5" width="22.9230769230769"/>
     <col collapsed="false" hidden="false" max="1025" min="26" style="1" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -46426,8 +46428,8 @@
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="47" width="9"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="48" width="31.17004048583"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="49" width="31.9230769230769"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="48" width="31.4939271255061"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="49" width="32.1376518218623"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -47290,14 +47292,14 @@
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="49" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="49" width="39.2064777327935"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="47" width="26.7813765182186"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="47" width="26.3522267206478"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="49" width="39.5263157894737"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="47" width="26.995951417004"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="47" width="26.5668016194332"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="47" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.4210526315789"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.5303643724696"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="30.6356275303644"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.6396761133603"/>
     <col collapsed="false" hidden="false" max="9" min="8" style="0" width="10.7125506072875"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="23.3522267206478"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="23.4574898785425"/>
     <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -55445,10 +55447,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.8866396761134"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.1012145748988"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.5668016194332"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.4210526315789"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.995951417004"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="21.2105263157895"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="23.6720647773279"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="27.6356275303644"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -55491,8 +55493,8 @@
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="47" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.6720647773279"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="47" width="18.4251012145749"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="35.9919028340081"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="47" width="18.5303643724696"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -55531,10 +55533,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.9919028340081"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.4574898785425"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="33.2064777327935"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="32.6720647773279"/>
     <col collapsed="false" hidden="false" max="5" min="3" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.17004048583"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="31.4939271255061"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -55674,7 +55676,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="44.1336032388664"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="44.4534412955466"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
PROS-10002 - MARSRU - Wrong KPI calculation
</commit_message>
<xml_diff>
--- a/Projects/MARSRU_PROD/Data/2019/MARS KPIs.xlsx
+++ b/Projects/MARSRU_PROD/Data/2019/MARS KPIs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs_Grocery" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
     <definedName function="false" hidden="true" localSheetId="5" name="_xlnm._FilterDatabase" vbProcedure="false">'4254'!$A$1:$J$259</definedName>
     <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">KPIs_Drogerie!$A$1:$AC$27</definedName>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">KPIs_Grocery!$A$1:$AC$63</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">KPIs_Grocery!$A$1:$AC$56</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">KPIs_Grocery!$A$1:$AC$63</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">KPIs_Grocery!$A$1:$AC$56</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">KPIs_Grocery!$A$1:$AC$56</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">KPIs_Grocery!$A$1:$AC$56</definedName>
@@ -39,6 +39,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs_Grocery!$A$1:$AC$56</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs_Grocery!$A$1:$AC$56</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs_Grocery!$A$1:$AC$56</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs_Grocery!$A$1:$AC$56</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_FilterDatabase_0" vbProcedure="false">KPIs_Drogerie!$B$1:$AC$1</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_FilterDatabase_0_0" vbProcedure="false">KPIs_Drogerie!$B$1:$AC$1</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_FilterDatabase_0_0_0" vbProcedure="false">KPIs_Drogerie!$B$1:$AC$1</definedName>
@@ -57,17 +58,17 @@
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AC$27</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AC$27</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AC$27</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AC$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AC$27</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AC$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AC$27</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AC$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AC$27</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AC$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AC$27</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AC$3</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AC$27</definedName>
-    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AC$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AC$27</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AC$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AC$27</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AC$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AC$27</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AC$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AC$27</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AC$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AC$27</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AC$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AC$27</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AC$3</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AC$3</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AC$3</definedName>
@@ -92,6 +93,7 @@
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AC$3</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AC$3</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AC$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPIs_Drogerie!$A$1:$AC$3</definedName>
     <definedName function="false" hidden="false" localSheetId="3" name="_xlnm._FilterDatabase" vbProcedure="false">'4317'!$A$1:$C$54</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase" vbProcedure="false">'4254'!$A$1:$J$259</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0" vbProcedure="false">'4254'!$A$1:$J$259</definedName>
@@ -119,10 +121,11 @@
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'4254'!$A$1:$J$259</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'4254'!$A$1:$J$259</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'4254'!$A$1:$J$259</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'4254'!$A$2:$J$260</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'4254'!$A$1:$J$259</definedName>
-    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'4254'!$A$2:$J$260</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'4254'!$A$1:$J$259</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'4254'!$A$2:$J$260</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'4254'!$A$1:$J$259</definedName>
     <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'4254'!$A$2:$J$260</definedName>
+    <definedName function="false" hidden="false" localSheetId="5" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'4254'!$A$2:$J$260</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -1793,29 +1796,31 @@
   <dimension ref="A1:AC63"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="K56" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="K1" activeCellId="0" sqref="K1"/>
-      <selection pane="bottomLeft" activeCell="A56" activeCellId="0" sqref="A56"/>
-      <selection pane="bottomRight" activeCell="K23" activeCellId="0" sqref="K23"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="O22" activeCellId="0" sqref="O22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="2" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="2" width="23.2429149797571"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="2" width="23.3522267206478"/>
     <col collapsed="false" hidden="false" max="7" min="5" style="2" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="30.6356275303644"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="106.477732793522"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="2" width="74.6599190283401"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="31.4939271255061"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="30.8502024291498"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="107.441295546559"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="2" width="75.3036437246964"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="31.7085020242915"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="2" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="16" min="13" style="2" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="3" width="38.2429149797571"/>
+    <col collapsed="false" hidden="false" max="14" min="13" style="2" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="2" width="19.9878542510121"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="2" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="3" width="38.5627530364372"/>
     <col collapsed="false" hidden="false" max="18" min="18" style="3" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="19" min="19" style="2" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="2" width="21.7449392712551"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="2" width="21.9595141700405"/>
     <col collapsed="false" hidden="false" max="29" min="21" style="2" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="1025" min="30" style="1" width="9.10526315789474"/>
   </cols>
@@ -1950,7 +1955,9 @@
       <c r="N2" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="O2" s="10"/>
+      <c r="O2" s="10" t="n">
+        <v>1</v>
+      </c>
       <c r="P2" s="10" t="n">
         <v>2</v>
       </c>
@@ -2013,7 +2020,9 @@
       <c r="N3" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="O3" s="10"/>
+      <c r="O3" s="10" t="n">
+        <v>1</v>
+      </c>
       <c r="P3" s="10" t="n">
         <v>2</v>
       </c>
@@ -3043,7 +3052,9 @@
       <c r="N19" s="10" t="n">
         <v>776682</v>
       </c>
-      <c r="O19" s="10"/>
+      <c r="O19" s="10" t="n">
+        <v>1</v>
+      </c>
       <c r="P19" s="10" t="n">
         <v>8</v>
       </c>
@@ -3100,7 +3111,9 @@
       <c r="N20" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="O20" s="10"/>
+      <c r="O20" s="10" t="n">
+        <v>0</v>
+      </c>
       <c r="P20" s="10"/>
       <c r="Q20" s="13" t="s">
         <v>85</v>
@@ -3159,7 +3172,9 @@
       <c r="N21" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="O21" s="10"/>
+      <c r="O21" s="10" t="n">
+        <v>0</v>
+      </c>
       <c r="P21" s="10"/>
       <c r="Q21" s="13" t="s">
         <v>88</v>
@@ -3218,7 +3233,9 @@
       <c r="N22" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="O22" s="10"/>
+      <c r="O22" s="10" t="n">
+        <v>1</v>
+      </c>
       <c r="P22" s="10"/>
       <c r="Q22" s="13" t="s">
         <v>91</v>
@@ -4436,7 +4453,9 @@
       <c r="N42" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="O42" s="10"/>
+      <c r="O42" s="10" t="n">
+        <v>0</v>
+      </c>
       <c r="P42" s="10"/>
       <c r="Q42" s="15" t="s">
         <v>140</v>
@@ -4495,7 +4514,9 @@
       <c r="N43" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="O43" s="10"/>
+      <c r="O43" s="10" t="n">
+        <v>0</v>
+      </c>
       <c r="P43" s="10"/>
       <c r="Q43" s="13" t="s">
         <v>143</v>
@@ -4554,7 +4575,9 @@
       <c r="N44" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="O44" s="10"/>
+      <c r="O44" s="10" t="n">
+        <v>1</v>
+      </c>
       <c r="P44" s="10"/>
       <c r="Q44" s="13" t="s">
         <v>147</v>
@@ -4617,7 +4640,9 @@
       <c r="N45" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="O45" s="10"/>
+      <c r="O45" s="10" t="n">
+        <v>1</v>
+      </c>
       <c r="P45" s="10"/>
       <c r="Q45" s="13" t="s">
         <v>153</v>
@@ -4676,7 +4701,9 @@
       <c r="N46" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="O46" s="10"/>
+      <c r="O46" s="10" t="n">
+        <v>1</v>
+      </c>
       <c r="P46" s="10"/>
       <c r="Q46" s="13" t="s">
         <v>91</v>
@@ -4735,7 +4762,9 @@
       <c r="N47" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="O47" s="10"/>
+      <c r="O47" s="10" t="n">
+        <v>1</v>
+      </c>
       <c r="P47" s="10"/>
       <c r="Q47" s="10" t="s">
         <v>159</v>
@@ -4796,7 +4825,9 @@
       <c r="N48" s="10" t="n">
         <v>3</v>
       </c>
-      <c r="O48" s="10"/>
+      <c r="O48" s="10" t="n">
+        <v>1</v>
+      </c>
       <c r="P48" s="10"/>
       <c r="Q48" s="10" t="s">
         <v>166</v>
@@ -4855,7 +4886,9 @@
       <c r="N49" s="10" t="n">
         <v>3</v>
       </c>
-      <c r="O49" s="10"/>
+      <c r="O49" s="10" t="n">
+        <v>1</v>
+      </c>
       <c r="P49" s="10"/>
       <c r="Q49" s="10" t="s">
         <v>170</v>
@@ -4918,7 +4951,9 @@
       <c r="N50" s="10" t="n">
         <v>3</v>
       </c>
-      <c r="O50" s="10"/>
+      <c r="O50" s="10" t="n">
+        <v>1</v>
+      </c>
       <c r="P50" s="10"/>
       <c r="Q50" s="10" t="s">
         <v>173</v>
@@ -4981,7 +5016,9 @@
       <c r="N51" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="O51" s="10"/>
+      <c r="O51" s="10" t="n">
+        <v>1</v>
+      </c>
       <c r="P51" s="10" t="n">
         <v>1</v>
       </c>
@@ -5044,7 +5081,9 @@
       <c r="N52" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="O52" s="10"/>
+      <c r="O52" s="10" t="n">
+        <v>1</v>
+      </c>
       <c r="P52" s="10" t="n">
         <v>1</v>
       </c>
@@ -5734,8 +5773,8 @@
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="19" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="43.3846153846154"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="21.2105263157895"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="43.7044534412956"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="21.3157894736842"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -5774,10 +5813,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="39.8502024291498"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="38.9919028340081"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="40.17004048583"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="39.3117408906883"/>
     <col collapsed="false" hidden="false" max="5" min="3" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="37.4898785425101"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="37.7044534412955"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -5917,7 +5956,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="53.668016194332"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="54.0931174089069"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -5975,7 +6014,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="true">
+  <sheetPr filterMode="false">
     <tabColor rgb="FFCCFF00"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -5986,26 +6025,26 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="K1" activeCellId="0" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L13" activeCellId="0" sqref="L13"/>
+      <selection pane="bottomRight" activeCell="O24" activeCellId="0" sqref="O24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="2" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="2" width="23.2429149797571"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="19.1740890688259"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="2" width="23.3522267206478"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="19.3886639676113"/>
     <col collapsed="false" hidden="false" max="7" min="6" style="2" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="30.6356275303644"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="106.477732793522"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="2" width="74.6599190283401"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="31.4939271255061"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="30.8502024291498"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="2" width="107.441295546559"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="2" width="75.3036437246964"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="31.7085020242915"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="2" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="16" min="13" style="2" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="3" width="38.2429149797571"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="3" width="38.5627530364372"/>
     <col collapsed="false" hidden="false" max="18" min="18" style="3" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="19" min="19" style="2" width="13.497975708502"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="2" width="21.7449392712551"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="2" width="21.9595141700405"/>
     <col collapsed="false" hidden="false" max="29" min="21" style="2" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="1025" min="30" style="1" width="9.10526315789474"/>
   </cols>
@@ -6099,7 +6138,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="29.95" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="29.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="10"/>
       <c r="B2" s="10" t="n">
         <v>2019</v>
@@ -6138,7 +6177,9 @@
       <c r="N2" s="10" t="n">
         <v>3</v>
       </c>
-      <c r="O2" s="10"/>
+      <c r="O2" s="10" t="n">
+        <v>1</v>
+      </c>
       <c r="P2" s="10"/>
       <c r="Q2" s="10" t="s">
         <v>170</v>
@@ -6162,7 +6203,7 @@
       <c r="AB2" s="10"/>
       <c r="AC2" s="10"/>
     </row>
-    <row r="3" customFormat="false" ht="29.95" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="29.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="10"/>
       <c r="B3" s="10" t="n">
         <v>2019</v>
@@ -6201,7 +6242,9 @@
       <c r="N3" s="10" t="n">
         <v>3</v>
       </c>
-      <c r="O3" s="10"/>
+      <c r="O3" s="10" t="n">
+        <v>1</v>
+      </c>
       <c r="P3" s="10"/>
       <c r="Q3" s="10" t="s">
         <v>173</v>
@@ -6225,7 +6268,7 @@
       <c r="AB3" s="10"/>
       <c r="AC3" s="10"/>
     </row>
-    <row r="4" customFormat="false" ht="29.95" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="29.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="10"/>
       <c r="B4" s="10" t="n">
         <v>2019</v>
@@ -6282,7 +6325,7 @@
       <c r="AB4" s="10"/>
       <c r="AC4" s="10"/>
     </row>
-    <row r="5" customFormat="false" ht="29.95" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="29.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="10"/>
       <c r="B5" s="10" t="n">
         <v>2019</v>
@@ -6339,7 +6382,7 @@
       <c r="AB5" s="10"/>
       <c r="AC5" s="10"/>
     </row>
-    <row r="6" customFormat="false" ht="29.95" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="29.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="10"/>
       <c r="B6" s="10" t="n">
         <v>2019</v>
@@ -6396,7 +6439,7 @@
       <c r="AB6" s="10"/>
       <c r="AC6" s="10"/>
     </row>
-    <row r="7" customFormat="false" ht="29.95" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="29.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="10" t="n">
         <v>2261</v>
       </c>
@@ -6461,7 +6504,7 @@
       <c r="AB7" s="10"/>
       <c r="AC7" s="10"/>
     </row>
-    <row r="8" customFormat="false" ht="29.95" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="29.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="10" t="n">
         <v>2262</v>
       </c>
@@ -6524,7 +6567,7 @@
       <c r="AB8" s="10"/>
       <c r="AC8" s="10"/>
     </row>
-    <row r="9" customFormat="false" ht="29.95" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="29.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="10" t="n">
         <v>2265</v>
       </c>
@@ -6589,7 +6632,7 @@
       <c r="AB9" s="10"/>
       <c r="AC9" s="10"/>
     </row>
-    <row r="10" customFormat="false" ht="29.95" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="29.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="10" t="n">
         <v>2266</v>
       </c>
@@ -6652,7 +6695,7 @@
       <c r="AB10" s="10"/>
       <c r="AC10" s="10"/>
     </row>
-    <row r="11" customFormat="false" ht="29.95" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="29.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="10"/>
       <c r="B11" s="10" t="n">
         <v>2019</v>
@@ -6833,7 +6876,7 @@
       <c r="AB13" s="10"/>
       <c r="AC13" s="10"/>
     </row>
-    <row r="14" customFormat="false" ht="29.95" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="29.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="10"/>
       <c r="B14" s="10" t="n">
         <v>2019</v>
@@ -7331,7 +7374,7 @@
       <c r="AB21" s="10"/>
       <c r="AC21" s="10"/>
     </row>
-    <row r="22" customFormat="false" ht="29.95" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="29.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="10"/>
       <c r="B22" s="10" t="n">
         <v>2019</v>
@@ -7388,7 +7431,7 @@
       <c r="AB22" s="10"/>
       <c r="AC22" s="10"/>
     </row>
-    <row r="23" customFormat="false" ht="29.95" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="29.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="10"/>
       <c r="B23" s="10" t="n">
         <v>2019</v>
@@ -7445,7 +7488,7 @@
       <c r="AB23" s="10"/>
       <c r="AC23" s="10"/>
     </row>
-    <row r="24" customFormat="false" ht="29.95" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="29.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="10" t="n">
         <v>2316</v>
       </c>
@@ -7484,7 +7527,9 @@
       <c r="N24" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="O24" s="10"/>
+      <c r="O24" s="10" t="n">
+        <v>1</v>
+      </c>
       <c r="P24" s="10"/>
       <c r="Q24" s="13" t="s">
         <v>147</v>
@@ -7508,7 +7553,7 @@
       <c r="AB24" s="10"/>
       <c r="AC24" s="10"/>
     </row>
-    <row r="25" customFormat="false" ht="29.95" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="29.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="10" t="s">
         <v>229</v>
       </c>
@@ -7547,7 +7592,9 @@
       <c r="N25" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="O25" s="10"/>
+      <c r="O25" s="10" t="n">
+        <v>1</v>
+      </c>
       <c r="P25" s="10"/>
       <c r="Q25" s="13" t="s">
         <v>91</v>
@@ -7567,7 +7614,7 @@
       <c r="AB25" s="10"/>
       <c r="AC25" s="10"/>
     </row>
-    <row r="26" customFormat="false" ht="29.95" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="29.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="10"/>
       <c r="B26" s="10" t="n">
         <v>2019</v>
@@ -7624,7 +7671,7 @@
       <c r="AB26" s="10"/>
       <c r="AC26" s="10"/>
     </row>
-    <row r="27" customFormat="false" ht="29.95" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="29.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="10"/>
       <c r="B27" s="10" t="n">
         <v>2019</v>
@@ -7661,7 +7708,9 @@
       <c r="N27" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="O27" s="10"/>
+      <c r="O27" s="10" t="n">
+        <v>1</v>
+      </c>
       <c r="P27" s="10"/>
       <c r="Q27" s="10"/>
       <c r="R27" s="10"/>
@@ -7721,13 +7770,7 @@
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <autoFilter ref="A1:AC27">
-    <filterColumn colId="11">
-      <customFilters and="true">
-        <customFilter operator="equal" val="SKUs"/>
-      </customFilters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:AC27"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -7752,8 +7795,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="53.668016194332"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.3522267206478"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="54.0931174089069"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.4615384615385"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -7934,8 +7977,8 @@
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="19" width="9"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="20" width="37.4898785425101"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="21" width="38.2429149797571"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="20" width="37.7044534412955"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="21" width="38.5627530364372"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -8797,8 +8840,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="20" width="37.4898785425101"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="21" width="38.2429149797571"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="20" width="37.7044534412955"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="21" width="38.5627530364372"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -8867,14 +8910,14 @@
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="21" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="21" width="47.5627530364373"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="32.1376518218623"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="19" width="31.7085020242915"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="21" width="47.9878542510121"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="19" width="32.3481781376518"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="19" width="31.9230769230769"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="19" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="36.5263157894737"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="36.8502024291498"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="9" min="8" style="0" width="10.7125506072875"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="27.4210526315789"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="27.6356275303644"/>
     <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -18366,7 +18409,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.9230769230769"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.0323886639676"/>
     <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -18442,10 +18485,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.3157894736842"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.7449392712551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.8502024291498"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.7773279352227"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.5303643724696"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.9595141700405"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.0647773279352"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.9919028340081"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>

</xml_diff>